<commit_message>
searching removed companies and small renaming
</commit_message>
<xml_diff>
--- a/RPA Framework/reqests.xlsx
+++ b/RPA Framework/reqests.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="54">
   <si>
     <t>Id</t>
   </si>
@@ -177,6 +178,12 @@
   </si>
   <si>
     <t>chronological</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -507,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +632,7 @@
         <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -660,7 +667,7 @@
         <v>41</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -695,7 +702,7 @@
         <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -730,7 +737,7 @@
         <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -835,7 +842,7 @@
         <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -867,7 +874,7 @@
         <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -899,7 +906,7 @@
         <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -931,7 +938,7 @@
         <v>49</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1413,4 +1420,438 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>7845</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>223750</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4292</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>352792</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>2263</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>224236</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>5011</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>25009</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3:C12" r:id="rId2" display="boogh313@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>